<commit_message>
Post July 28 meeting
</commit_message>
<xml_diff>
--- a/misc_docs/tobacco_qualifier_to_pcornet_2.xlsx
+++ b/misc_docs/tobacco_qualifier_to_pcornet_2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\omop\ETL\pSCANNER\pCORnet CDM\working group\homework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\omop\ETL\pSCANNER\pCORnet CDM\working group\git\OMOPv5-to-PCORnetv3\misc_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13200" firstSheet="1" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13200" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4437" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4402" uniqueCount="171">
   <si>
     <t>Description</t>
   </si>
@@ -523,9 +523,6 @@
     <t>Possible PCORnet values</t>
   </si>
   <si>
-    <t>2 Hand</t>
-  </si>
-  <si>
     <t>Desc</t>
   </si>
   <si>
@@ -533,6 +530,15 @@
   </si>
   <si>
     <t>Proposed solution. Two step process 1) Quantify the possible observation codes into a list of components that are sufficient to answer the PCORnet questions. 2) Create a mapping from the possible quantified values to the pcornet codes.</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Second Hand</t>
+  </si>
+  <si>
+    <t>Second</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1045,7 @@
         <v>42532</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1049,15 +1055,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="78.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1077,10 +1084,10 @@
         <v>160</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="13" t="s">
@@ -1146,10 +1153,10 @@
         <v>161</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12" t="s">
@@ -1230,10 +1237,10 @@
         <v>162</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
@@ -1285,10 +1292,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C17" s="12">
         <v>4</v>
@@ -1300,10 +1307,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C18" s="12">
         <v>5</v>
@@ -1314,38 +1321,38 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
+      <c r="A19" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="12">
+        <v>6</v>
+      </c>
       <c r="D19" s="12"/>
       <c r="E19" s="12" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>167</v>
-      </c>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C21" s="12">
-        <v>1</v>
+      <c r="A21" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="12" t="s">
@@ -1354,13 +1361,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C22" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12" t="s">
@@ -1369,13 +1376,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C23" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12" t="s">
@@ -1383,36 +1390,36 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
+      <c r="A24" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="12">
+        <v>3</v>
+      </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>167</v>
-      </c>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="13" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" s="12">
-        <v>1</v>
+      <c r="A26" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12" t="s">
@@ -1421,13 +1428,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C27" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12" t="s">
@@ -1436,13 +1443,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C28" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12" t="s">
@@ -1451,13 +1458,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C29" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12" t="s">
@@ -1465,9 +1472,15 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
+      <c r="A30" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="12">
+        <v>4</v>
+      </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12" t="s">
         <v>122</v>
@@ -1499,6 +1512,11 @@
       <c r="E33" s="12" t="s">
         <v>110</v>
       </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2134,11 +2152,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,15 +2168,14 @@
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" customWidth="1"/>
-    <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="71.7109375" customWidth="1"/>
-    <col min="13" max="13" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="33" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="71.7109375" customWidth="1"/>
+    <col min="12" max="12" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>136</v>
       </c>
@@ -2180,24 +2197,21 @@
       <c r="G1" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="I1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="J1" s="6" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="L1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>59</v>
       </c>
@@ -2219,23 +2233,20 @@
       <c r="G2" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H2" t="s">
-        <v>126</v>
+      <c r="I2" t="s">
+        <v>106</v>
       </c>
       <c r="J2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="K2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L2" t="s">
         <v>122</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>77</v>
       </c>
@@ -2257,23 +2268,20 @@
       <c r="G3" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>126</v>
+      <c r="I3" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L3" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>71</v>
       </c>
@@ -2295,23 +2303,20 @@
       <c r="G4" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>126</v>
+      <c r="I4" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L4" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="L4" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>73</v>
       </c>
@@ -2333,23 +2338,20 @@
       <c r="G5" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>126</v>
+      <c r="I5" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="L5" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>30</v>
       </c>
@@ -2371,23 +2373,20 @@
       <c r="G6" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>126</v>
+      <c r="I6" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L6" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="L6" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
@@ -2409,23 +2408,20 @@
       <c r="G7" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>126</v>
+      <c r="I7" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L7" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="L7" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -2447,23 +2443,20 @@
       <c r="G8" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>126</v>
+      <c r="I8" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L8" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="L8" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
@@ -2485,23 +2478,20 @@
       <c r="G9" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>126</v>
+      <c r="I9" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L9" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="L9" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
@@ -2523,23 +2513,20 @@
       <c r="G10" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>126</v>
+      <c r="I10" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L10" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="L10" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>22</v>
       </c>
@@ -2561,23 +2548,20 @@
       <c r="G11" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>126</v>
+      <c r="I11" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L11" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="L11" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
@@ -2599,23 +2583,20 @@
       <c r="G12" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>126</v>
+      <c r="I12" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L12" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="L12" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
@@ -2637,23 +2618,20 @@
       <c r="G13" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>126</v>
+      <c r="I13" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M13" s="12" t="s">
+      <c r="L13" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>4</v>
       </c>
@@ -2675,21 +2653,18 @@
       <c r="G14" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>126</v>
+      <c r="I14" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L14" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M14" s="12"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>34</v>
       </c>
@@ -2711,23 +2686,20 @@
       <c r="G15" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>126</v>
+      <c r="I15" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L15" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M15" s="13" t="s">
+      <c r="L15" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>16</v>
       </c>
@@ -2749,23 +2721,20 @@
       <c r="G16" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>126</v>
+      <c r="I16" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L16" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M16" s="12" t="s">
+      <c r="L16" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>10</v>
       </c>
@@ -2787,23 +2756,20 @@
       <c r="G17" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>126</v>
+      <c r="I17" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L17" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="M17" s="12" t="s">
+      <c r="L17" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>24</v>
       </c>
@@ -2825,23 +2791,20 @@
       <c r="G18" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>126</v>
+      <c r="I18" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="K18" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L18" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>41</v>
       </c>
@@ -2863,23 +2826,20 @@
       <c r="G19" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>126</v>
+      <c r="I19" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L19" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M19" s="12" t="s">
+      <c r="L19" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>55</v>
       </c>
@@ -2901,23 +2861,20 @@
       <c r="G20" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>126</v>
+      <c r="I20" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L20" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M20" s="12" t="s">
+      <c r="L20" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>67</v>
       </c>
@@ -2939,23 +2896,20 @@
       <c r="G21" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>126</v>
+      <c r="I21" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L21" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M21" s="12" t="s">
+      <c r="L21" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>97</v>
       </c>
@@ -2977,23 +2931,20 @@
       <c r="G22" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>126</v>
+      <c r="I22" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="K22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L22" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="L22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>37</v>
       </c>
@@ -3015,23 +2966,20 @@
       <c r="G23" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>126</v>
+      <c r="I23" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M23" s="12" t="s">
+      <c r="L23" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>51</v>
       </c>
@@ -3053,21 +3001,18 @@
       <c r="G24" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>126</v>
+      <c r="I24" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L24" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M24" s="12"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L24" s="12"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>65</v>
       </c>
@@ -3089,23 +3034,20 @@
       <c r="G25" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>126</v>
+      <c r="I25" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L25" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M25" s="13" t="s">
+      <c r="L25" s="13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>39</v>
       </c>
@@ -3127,23 +3069,20 @@
       <c r="G26" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>126</v>
+      <c r="I26" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L26" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M26" s="12" t="s">
+      <c r="L26" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>53</v>
       </c>
@@ -3165,23 +3104,20 @@
       <c r="G27" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>126</v>
+      <c r="I27" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L27" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M27" s="12" t="s">
+      <c r="L27" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>12</v>
       </c>
@@ -3203,23 +3139,20 @@
       <c r="G28" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>126</v>
+      <c r="I28" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="L28" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M28" s="12" t="s">
+      <c r="L28" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>14</v>
       </c>
@@ -3241,23 +3174,20 @@
       <c r="G29" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>126</v>
+      <c r="I29" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="L29" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="M29" s="12" t="s">
+      <c r="L29" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>8</v>
       </c>
@@ -3279,23 +3209,20 @@
       <c r="G30" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>126</v>
+      <c r="I30" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="L30" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M30" s="12" t="s">
+      <c r="L30" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>32</v>
       </c>
@@ -3317,23 +3244,20 @@
       <c r="G31" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>126</v>
+      <c r="I31" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="L31" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="M31" s="12" t="s">
+      <c r="L31" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>49</v>
       </c>
@@ -3355,23 +3279,20 @@
       <c r="G32" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>126</v>
+      <c r="I32" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L32" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M32" s="12" t="s">
+      <c r="L32" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>63</v>
       </c>
@@ -3393,23 +3314,20 @@
       <c r="G33" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>126</v>
+      <c r="I33" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L33" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M33" s="12" t="s">
+      <c r="L33" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>92</v>
       </c>
@@ -3431,20 +3349,17 @@
       <c r="G34" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>126</v>
+      <c r="I34" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="L34" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>79</v>
       </c>
@@ -3466,20 +3381,17 @@
       <c r="G35" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>126</v>
+      <c r="I35" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L35" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>75</v>
       </c>
@@ -3501,20 +3413,17 @@
       <c r="G36" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>126</v>
+      <c r="I36" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L36" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>69</v>
       </c>
@@ -3536,20 +3445,17 @@
       <c r="G37" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>126</v>
+      <c r="I37" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L37" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>45</v>
       </c>
@@ -3571,20 +3477,17 @@
       <c r="G38" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>126</v>
+      <c r="I38" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L38" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>61</v>
       </c>
@@ -3606,20 +3509,17 @@
       <c r="G39" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>126</v>
+      <c r="I39" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L39" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>47</v>
       </c>
@@ -3641,20 +3541,17 @@
       <c r="G40" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>126</v>
+      <c r="I40" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L40" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>43</v>
       </c>
@@ -3676,20 +3573,17 @@
       <c r="G41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>126</v>
+      <c r="I41" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L41" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>57</v>
       </c>
@@ -3711,20 +3605,17 @@
       <c r="G42" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>126</v>
+      <c r="I42" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L42" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>4009853</v>
       </c>
@@ -3738,7 +3629,7 @@
         <v>126</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>126</v>
+        <v>168</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>126</v>
@@ -3746,29 +3637,26 @@
       <c r="G43" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>127</v>
+      <c r="I43" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="L43" s="2" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I43">
+      <formula1>$L$3:$L$13</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J43">
-      <formula1>$M$3:$M$13</formula1>
+      <formula1>$L$16:$L$23</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K43">
-      <formula1>$M$16:$M$23</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L43">
-      <formula1>$M$26:$M$33</formula1>
+      <formula1>$L$26:$L$33</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3789,15 +3677,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Complete map'!$K$52:$K$56</xm:f>
+            <xm:f>'Complete map'!$K$36:$K$38</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E43</xm:sqref>
+          <xm:sqref>C2:C43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Complete map'!$K$36:$K$38</xm:f>
+            <xm:f>'Complete map'!$K$52:$K$57</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C43</xm:sqref>
+          <xm:sqref>E2:E43</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3810,8 +3698,8 @@
   <dimension ref="A1:M721"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:E1"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5523,6 +5411,9 @@
       <c r="K52" t="s">
         <v>134</v>
       </c>
+      <c r="L52" t="s">
+        <v>154</v>
+      </c>
       <c r="M52">
         <v>1</v>
       </c>
@@ -5558,6 +5449,9 @@
       <c r="K53" t="s">
         <v>130</v>
       </c>
+      <c r="L53" t="s">
+        <v>156</v>
+      </c>
       <c r="M53">
         <v>2</v>
       </c>
@@ -5593,6 +5487,9 @@
       <c r="K54" t="s">
         <v>135</v>
       </c>
+      <c r="L54" t="s">
+        <v>157</v>
+      </c>
       <c r="M54">
         <v>3</v>
       </c>
@@ -5625,10 +5522,13 @@
         <f t="shared" si="2"/>
         <v>03=Use of both smoked and non-smoked tobacco products</v>
       </c>
-      <c r="K55" t="s">
-        <v>131</v>
-      </c>
-      <c r="M55">
+      <c r="K55" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="M55" s="2">
         <v>4</v>
       </c>
     </row>
@@ -5661,10 +5561,10 @@
         <v>01=Smoked tobacco only</v>
       </c>
       <c r="K56" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="L56" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="M56">
         <v>5</v>
@@ -5697,6 +5597,15 @@
       <c r="I57" s="3" t="str">
         <f t="shared" si="2"/>
         <v>01=Smoked tobacco only</v>
+      </c>
+      <c r="K57" t="s">
+        <v>126</v>
+      </c>
+      <c r="L57" t="s">
+        <v>144</v>
+      </c>
+      <c r="M57">
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>